<commit_message>
mutual fund filter updated
</commit_message>
<xml_diff>
--- a/桌面/抗通胀/流程额度.xlsx
+++ b/桌面/抗通胀/流程额度.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\工作电脑\桌面\抗通胀\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8C896D-A3EB-47E4-B377-79FE032DBC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932F05D6-377A-46D9-BDBB-95EA40267410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="381">
   <si>
     <t>代码</t>
   </si>
@@ -1235,6 +1235,26 @@
   </si>
   <si>
     <t>安信稳健增利</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>招商安华A/C</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>008791.OF</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>鹏华双债增利</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>000054.OF</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>二级债基</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1895,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3118,6 +3138,48 @@
         <v>300</v>
       </c>
       <c r="G49" s="2">
+        <v>44561</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D50" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F50">
+        <f>D50-E50</f>
+        <v>1000</v>
+      </c>
+      <c r="G50" s="2">
+        <v>44561</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F51">
+        <f>D51-E51</f>
+        <v>1000</v>
+      </c>
+      <c r="G51" s="2">
         <v>44561</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some changes in account
</commit_message>
<xml_diff>
--- a/桌面/抗通胀/流程额度.xlsx
+++ b/桌面/抗通胀/流程额度.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\工作电脑\桌面\抗通胀\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932F05D6-377A-46D9-BDBB-95EA40267410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B565A9D-05BC-4BDC-8C40-602BA09CCFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1915,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2920,11 +2920,11 @@
         <v>2000</v>
       </c>
       <c r="E40">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G40" s="2">
         <v>44561</v>

</xml_diff>

<commit_message>
some updates in fund filtering
</commit_message>
<xml_diff>
--- a/桌面/抗通胀/流程额度.xlsx
+++ b/桌面/抗通胀/流程额度.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\工作电脑\桌面\抗通胀\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA532959-4E83-4BF5-BCC8-B34353FFD6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5BC288-8DD6-4E88-9D8F-16CB893F3A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="384">
   <si>
     <t>代码</t>
   </si>
@@ -1255,6 +1255,18 @@
   </si>
   <si>
     <t>二级债基</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>上投摩根医疗健康</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票基金</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>001766.OF</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1915,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3177,6 +3189,30 @@
         <v>1000</v>
       </c>
       <c r="G51" s="2">
+        <v>44561</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="D52" s="4">
+        <v>500</v>
+      </c>
+      <c r="E52">
+        <v>200</v>
+      </c>
+      <c r="F52">
+        <f>D52-E52</f>
+        <v>300</v>
+      </c>
+      <c r="G52" s="2">
         <v>44561</v>
       </c>
     </row>

</xml_diff>